<commit_message>
Dividing the code into categories
</commit_message>
<xml_diff>
--- a/20210919_county_facts_dictionary.xlsx
+++ b/20210919_county_facts_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doria\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Desktop\ISA\projekt_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7151D9A2-A0D8-4FF9-890C-D9F28DB91F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{33A156FE-443F-4E39-A772-267C44C334B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="county_facts_dictionary (2)" sheetId="2" r:id="rId1"/>
@@ -19,20 +19,21 @@
   <definedNames>
     <definedName name="DaneZewnętrzne_1" localSheetId="0" hidden="1">'county_facts_dictionary (2)'!$A$1:$B$53</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Zapytanie — county_facts_dictionary" description="Połączenie z zapytaniem „county_facts_dictionary” w skoroszycie." type="5" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Zapytanie — county_facts_dictionary" description="Połączenie z zapytaniem „county_facts_dictionary” w skoroszycie." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=county_facts_dictionary;Extended Properties=&quot;&quot;" command="SELECT * FROM [county_facts_dictionary]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="175">
   <si>
     <t>column_name,description</t>
   </si>
@@ -554,12 +555,15 @@
   </si>
   <si>
     <t>biznes</t>
+  </si>
+  <si>
+    <t>populacje/wiek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1134,7 +1138,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
@@ -1146,12 +1150,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="county_facts_dictionary" displayName="county_facts_dictionary" ref="A1:C53" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="county_facts_dictionary" displayName="county_facts_dictionary" ref="A1:C53" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="2" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="1"/>
-    <tableColumn id="3" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1453,21 +1457,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:C50"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.5546875" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1478,7 +1482,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
@@ -1489,7 +1493,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -1500,7 +1504,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1511,7 +1515,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -1522,7 +1526,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
@@ -1533,7 +1537,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
@@ -1541,10 +1545,10 @@
         <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>66</v>
       </c>
@@ -1552,10 +1556,10 @@
         <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
@@ -1563,10 +1567,10 @@
         <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
@@ -1577,7 +1581,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>72</v>
       </c>
@@ -1588,7 +1592,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>74</v>
       </c>
@@ -1599,7 +1603,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1610,7 +1614,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -1621,7 +1625,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>80</v>
       </c>
@@ -1632,7 +1636,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -1643,7 +1647,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>84</v>
       </c>
@@ -1654,7 +1658,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>86</v>
       </c>
@@ -1665,7 +1669,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
@@ -1676,7 +1680,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>90</v>
       </c>
@@ -1687,7 +1691,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>92</v>
       </c>
@@ -1698,7 +1702,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>94</v>
       </c>
@@ -1709,7 +1713,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
@@ -1720,7 +1724,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>98</v>
       </c>
@@ -1731,7 +1735,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>100</v>
       </c>
@@ -1742,7 +1746,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>102</v>
       </c>
@@ -1753,7 +1757,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>104</v>
       </c>
@@ -1764,7 +1768,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>106</v>
       </c>
@@ -1775,7 +1779,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>108</v>
       </c>
@@ -1786,7 +1790,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>110</v>
       </c>
@@ -1797,7 +1801,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>112</v>
       </c>
@@ -1808,7 +1812,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>114</v>
       </c>
@@ -1819,7 +1823,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>116</v>
       </c>
@@ -1830,7 +1834,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>118</v>
       </c>
@@ -1841,7 +1845,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>120</v>
       </c>
@@ -1855,7 +1859,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>122</v>
       </c>
@@ -1866,7 +1870,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>124</v>
       </c>
@@ -1877,7 +1881,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>126</v>
       </c>
@@ -1888,7 +1892,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>128</v>
       </c>
@@ -1899,7 +1903,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>130</v>
       </c>
@@ -1910,7 +1914,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>132</v>
       </c>
@@ -1921,7 +1925,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>134</v>
       </c>
@@ -1932,7 +1936,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>136</v>
       </c>
@@ -1943,7 +1947,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>138</v>
       </c>
@@ -1954,7 +1958,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>140</v>
       </c>
@@ -1965,7 +1969,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>142</v>
       </c>
@@ -1976,7 +1980,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>144</v>
       </c>
@@ -1987,7 +1991,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>146</v>
       </c>
@@ -1998,7 +2002,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>148</v>
       </c>
@@ -2009,7 +2013,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>150</v>
       </c>
@@ -2020,7 +2024,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>152</v>
       </c>
@@ -2031,7 +2035,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>154</v>
       </c>
@@ -2042,7 +2046,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>156</v>
       </c>
@@ -2062,269 +2066,269 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>

</xml_diff>